<commit_message>
read xlsx & write map ok
</commit_message>
<xml_diff>
--- a/16_03_sendDuesReminders/duesRecords.xlsx
+++ b/16_03_sendDuesReminders/duesRecords.xlsx
@@ -8,12 +8,12 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -95,11 +95,9 @@
   </numFmts>
   <fonts count="5">
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -167,12 +165,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -196,17 +198,15 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -232,151 +232,151 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="0" t="s">
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
+    <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>